<commit_message>
data towers und projectiles added
</commit_message>
<xml_diff>
--- a/Tower-Data.xlsx
+++ b/Tower-Data.xlsx
@@ -256,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -381,11 +381,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -400,6 +411,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -682,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1980,7 +1992,7 @@
         <v>8</v>
       </c>
       <c r="F31" s="2">
-        <v>1666</v>
+        <v>1616</v>
       </c>
       <c r="G31" s="2">
         <v>64</v>
@@ -1993,51 +2005,51 @@
       </c>
       <c r="K31">
         <f>E31*(1000/F31)</f>
-        <v>4.8019207683073226</v>
+        <v>4.9504950495049505</v>
       </c>
       <c r="L31">
         <f>K31/D31</f>
-        <v>2.4009603841536612E-2</v>
+        <v>2.4752475247524754E-2</v>
       </c>
       <c r="N31">
         <f>AA31/(K31)</f>
-        <v>2.9155000000000002</v>
+        <v>2.8279999999999998</v>
       </c>
       <c r="O31">
         <f>AA32/K31</f>
-        <v>7.2887500000000003</v>
+        <v>7.07</v>
       </c>
       <c r="P31">
         <f>AA33/K31</f>
-        <v>20.825000000000003</v>
+        <v>20.2</v>
       </c>
       <c r="Q31">
         <f>AA34/(K31/3)</f>
-        <v>12.495000000000001</v>
+        <v>12.120000000000001</v>
       </c>
       <c r="R31">
         <f>AA35/K31</f>
-        <v>9.3712499999999999</v>
+        <v>9.09</v>
       </c>
       <c r="S31">
         <f>AA36/K31</f>
-        <v>31.237500000000001</v>
+        <v>30.3</v>
       </c>
       <c r="T31">
         <f>AA37/(K31/3)</f>
-        <v>12.495000000000001</v>
+        <v>12.120000000000001</v>
       </c>
       <c r="U31">
         <f>AA38/(K31/3)</f>
-        <v>15.61875</v>
+        <v>15.15</v>
       </c>
       <c r="V31">
         <f>AA39/K31</f>
-        <v>52.0625</v>
+        <v>50.5</v>
       </c>
       <c r="W31">
         <f>AA40/(K31/3)</f>
-        <v>21.866250000000001</v>
+        <v>21.21</v>
       </c>
       <c r="Z31" s="10" t="s">
         <v>32</v>
@@ -2066,10 +2078,10 @@
         <v>450</v>
       </c>
       <c r="E32" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F32" s="2">
-        <v>1388</v>
+        <v>1338</v>
       </c>
       <c r="G32" s="2">
         <v>72</v>
@@ -2082,51 +2094,51 @@
       </c>
       <c r="K32">
         <f>E32*(1000/F32)</f>
-        <v>7.2046109510086449</v>
+        <v>8.2212257100149468</v>
       </c>
       <c r="L32">
         <f>K32/D32</f>
-        <v>1.6010246557796988E-2</v>
+        <v>1.8269390466699884E-2</v>
       </c>
       <c r="N32">
         <f>AA31/K32</f>
-        <v>1.9432000000000003</v>
+        <v>1.7029090909090911</v>
       </c>
       <c r="O32">
         <f>AA32/K32</f>
-        <v>4.8580000000000005</v>
+        <v>4.2572727272727278</v>
       </c>
       <c r="P32">
         <f>AA33/K32</f>
-        <v>13.88</v>
+        <v>12.163636363636364</v>
       </c>
       <c r="Q32">
         <f>AA34/(K32/3)</f>
-        <v>8.3280000000000012</v>
+        <v>7.2981818181818188</v>
       </c>
       <c r="R32">
         <f>AA35/K32</f>
-        <v>6.2460000000000004</v>
+        <v>5.4736363636363645</v>
       </c>
       <c r="S32">
         <f>AA36/K32</f>
-        <v>20.82</v>
+        <v>18.245454545454546</v>
       </c>
       <c r="T32">
         <f>AA37/(K32/3)</f>
-        <v>8.3280000000000012</v>
+        <v>7.2981818181818188</v>
       </c>
       <c r="U32">
         <f>AA38/(K32/3)</f>
-        <v>10.410000000000002</v>
+        <v>9.122727272727273</v>
       </c>
       <c r="V32">
         <f>AA39/K32</f>
-        <v>34.700000000000003</v>
+        <v>30.409090909090914</v>
       </c>
       <c r="W32">
         <f>AA40/(K32/3)</f>
-        <v>14.574000000000002</v>
+        <v>12.771818181818183</v>
       </c>
       <c r="Z32" s="2" t="s">
         <v>47</v>
@@ -2155,10 +2167,10 @@
         <v>750</v>
       </c>
       <c r="E33" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F33" s="2">
-        <v>1190</v>
+        <v>1140</v>
       </c>
       <c r="G33" s="2">
         <v>80</v>
@@ -2171,51 +2183,51 @@
       </c>
       <c r="K33">
         <f>E33*(1000/F33)</f>
-        <v>10.084033613445378</v>
+        <v>12.280701754385964</v>
       </c>
       <c r="L33">
         <f>K33/D33</f>
-        <v>1.3445378151260503E-2</v>
+        <v>1.6374269005847951E-2</v>
       </c>
       <c r="N33">
         <f>AA31/K33</f>
-        <v>1.3883333333333334</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="O33">
         <f>AA32/K33</f>
-        <v>3.4708333333333332</v>
+        <v>2.85</v>
       </c>
       <c r="P33">
         <f>AA33/K33</f>
-        <v>9.9166666666666661</v>
+        <v>8.1428571428571441</v>
       </c>
       <c r="Q33">
         <f>AA34/(K33/3)</f>
-        <v>5.95</v>
+        <v>4.8857142857142861</v>
       </c>
       <c r="R33">
         <f>AA35/K33</f>
-        <v>4.4625000000000004</v>
+        <v>3.6642857142857146</v>
       </c>
       <c r="S33">
         <f>AA36/K33</f>
-        <v>14.875</v>
+        <v>12.214285714285715</v>
       </c>
       <c r="T33">
         <f>AA37/(K33/3)</f>
-        <v>5.95</v>
+        <v>4.8857142857142861</v>
       </c>
       <c r="U33">
         <f>AA38/(K33/3)</f>
-        <v>7.4375</v>
+        <v>6.1071428571428568</v>
       </c>
       <c r="V33">
         <f>AA39/K33</f>
-        <v>24.791666666666668</v>
+        <v>20.357142857142858</v>
       </c>
       <c r="W33">
         <f>AA40/(K33/3)</f>
-        <v>10.4125</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="Z33" s="2" t="s">
         <v>33</v>
@@ -2246,10 +2258,10 @@
         <v>1100</v>
       </c>
       <c r="E34" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F34" s="2">
-        <v>1041</v>
+        <v>991</v>
       </c>
       <c r="G34" s="2">
         <v>88</v>
@@ -2262,51 +2274,51 @@
       </c>
       <c r="K34">
         <f>E34*(1000/F34)</f>
-        <v>13.448607108549472</v>
+        <v>17.15438950554995</v>
       </c>
       <c r="L34">
         <f>K34/D34</f>
-        <v>1.2226006462317703E-2</v>
+        <v>1.5594899550499955E-2</v>
       </c>
       <c r="N34">
         <f>AA31/K34</f>
-        <v>1.0409999999999999</v>
+        <v>0.8161176470588235</v>
       </c>
       <c r="O34">
         <f>AA32/K34</f>
-        <v>2.6025</v>
+        <v>2.0402941176470586</v>
       </c>
       <c r="P34">
         <f>AA33/K34</f>
-        <v>7.4357142857142851</v>
+        <v>5.8294117647058821</v>
       </c>
       <c r="Q34">
         <f>AA34/(K34/3)</f>
-        <v>4.4614285714285709</v>
+        <v>3.4976470588235293</v>
       </c>
       <c r="R34">
         <f>AA35/K34</f>
-        <v>3.3460714285714284</v>
+        <v>2.6232352941176469</v>
       </c>
       <c r="S34">
         <f>AA36/K34</f>
-        <v>11.153571428571428</v>
+        <v>8.7441176470588236</v>
       </c>
       <c r="T34">
         <f>AA37/(K34/3)</f>
-        <v>4.4614285714285709</v>
+        <v>3.4976470588235293</v>
       </c>
       <c r="U34">
         <f>AA38/(K34/3)</f>
-        <v>5.5767857142857133</v>
+        <v>4.3720588235294118</v>
       </c>
       <c r="V34">
         <f>AA39/K34</f>
-        <v>18.589285714285712</v>
+        <v>14.573529411764705</v>
       </c>
       <c r="W34">
         <f>AA40/(K34/3)</f>
-        <v>7.8074999999999992</v>
+        <v>6.1208823529411767</v>
       </c>
       <c r="Z34" s="2" t="s">
         <v>34</v>
@@ -2337,10 +2349,10 @@
         <v>1500</v>
       </c>
       <c r="E35" s="2">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F35" s="2">
-        <v>925</v>
+        <v>875</v>
       </c>
       <c r="G35" s="2">
         <v>96</v>
@@ -2353,51 +2365,51 @@
       </c>
       <c r="K35">
         <f>E35*(1000/F35)</f>
-        <v>17.297297297297298</v>
+        <v>22.857142857142854</v>
       </c>
       <c r="L35">
         <f>K35/D35</f>
-        <v>1.1531531531531532E-2</v>
+        <v>1.5238095238095236E-2</v>
       </c>
       <c r="N35">
         <f>AA31/K35</f>
-        <v>0.80937499999999996</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="O35">
         <f>AA32/K35</f>
-        <v>2.0234375</v>
+        <v>1.5312500000000002</v>
       </c>
       <c r="P35">
         <f>AA33/K35</f>
-        <v>5.78125</v>
+        <v>4.3750000000000009</v>
       </c>
       <c r="Q35">
         <f>AA34/(K35/3)</f>
-        <v>3.4687499999999996</v>
+        <v>2.6250000000000004</v>
       </c>
       <c r="R35">
         <f>AA35/K35</f>
-        <v>2.6015625</v>
+        <v>1.9687500000000002</v>
       </c>
       <c r="S35">
         <f>AA36/K35</f>
-        <v>8.671875</v>
+        <v>6.5625000000000009</v>
       </c>
       <c r="T35">
         <f>AA37/(K35/3)</f>
-        <v>3.4687499999999996</v>
+        <v>2.6250000000000004</v>
       </c>
       <c r="U35">
         <f>AA38/(K35/3)</f>
-        <v>4.3359374999999991</v>
+        <v>3.2812500000000004</v>
       </c>
       <c r="V35">
         <f>AA39/K35</f>
-        <v>14.453125</v>
+        <v>10.937500000000002</v>
       </c>
       <c r="W35">
         <f>AA40/(K35/3)</f>
-        <v>6.0703124999999991</v>
+        <v>4.5937500000000009</v>
       </c>
       <c r="Z35" s="2" t="s">
         <v>35</v>
@@ -2416,6 +2428,7 @@
       </c>
     </row>
     <row r="36" spans="2:30" x14ac:dyDescent="0.3">
+      <c r="E36" s="14"/>
       <c r="Z36" s="2" t="s">
         <v>36</v>
       </c>
@@ -2550,13 +2563,13 @@
         <v>170</v>
       </c>
       <c r="E50" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F50" s="2">
         <v>1000</v>
       </c>
       <c r="G50" s="2">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>25</v>
@@ -2566,51 +2579,51 @@
       </c>
       <c r="K50">
         <f>E50*(1000/F50)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L50">
         <f>K50/D50</f>
-        <v>1.1764705882352941E-2</v>
+        <v>1.7647058823529412E-2</v>
       </c>
       <c r="N50">
         <f>AA50/(K50)</f>
-        <v>7</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="O50">
         <f>AA51/K50</f>
-        <v>17.5</v>
+        <v>11.666666666666666</v>
       </c>
       <c r="P50">
         <f>AA52/K50</f>
-        <v>50</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="Q50">
         <f>AA53/(K50/3)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="R50">
         <f>AA54/K50</f>
-        <v>22.5</v>
+        <v>15</v>
       </c>
       <c r="S50">
         <f>AA55/K50</f>
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="T50">
         <f>AA56/(K50/3)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="U50">
         <f>AA57/(K50/3)</f>
-        <v>37.5</v>
+        <v>25</v>
       </c>
       <c r="V50">
         <f>AA58/K50</f>
-        <v>125</v>
+        <v>83.333333333333329</v>
       </c>
       <c r="W50">
         <f>AA59/(K50/3)</f>
-        <v>52.5</v>
+        <v>35</v>
       </c>
       <c r="Z50" s="10" t="s">
         <v>32</v>
@@ -2639,13 +2652,13 @@
         <v>390</v>
       </c>
       <c r="E51" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F51" s="2">
         <v>833</v>
       </c>
       <c r="G51" s="2">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>25</v>
@@ -2655,51 +2668,51 @@
       </c>
       <c r="K51">
         <f>E51*(1000/F51)</f>
-        <v>3.601440576230492</v>
+        <v>4.8019207683073226</v>
       </c>
       <c r="L51">
         <f>K51/D51</f>
-        <v>9.2344630159756202E-3</v>
+        <v>1.231261735463416E-2</v>
       </c>
       <c r="N51">
         <f>AA50/K51</f>
-        <v>3.8873333333333338</v>
+        <v>2.9155000000000002</v>
       </c>
       <c r="O51">
         <f>AA51/K51</f>
-        <v>9.7183333333333337</v>
+        <v>7.2887500000000003</v>
       </c>
       <c r="P51">
         <f>AA52/K51</f>
-        <v>27.766666666666669</v>
+        <v>20.825000000000003</v>
       </c>
       <c r="Q51">
         <f>AA53/(K51/3)</f>
-        <v>16.66</v>
+        <v>12.495000000000001</v>
       </c>
       <c r="R51">
         <f>AA54/K51</f>
-        <v>12.495000000000001</v>
+        <v>9.3712499999999999</v>
       </c>
       <c r="S51">
         <f>AA55/K51</f>
-        <v>41.650000000000006</v>
+        <v>31.237500000000001</v>
       </c>
       <c r="T51">
         <f>AA56/(K51/3)</f>
-        <v>16.66</v>
+        <v>12.495000000000001</v>
       </c>
       <c r="U51">
         <f>AA57/(K51/3)</f>
-        <v>20.825000000000003</v>
+        <v>15.61875</v>
       </c>
       <c r="V51">
         <f>AA58/K51</f>
-        <v>69.416666666666671</v>
+        <v>52.0625</v>
       </c>
       <c r="W51">
         <f>AA59/(K51/3)</f>
-        <v>29.155000000000001</v>
+        <v>21.866250000000001</v>
       </c>
       <c r="Z51" s="2" t="s">
         <v>47</v>
@@ -2728,13 +2741,13 @@
         <v>660</v>
       </c>
       <c r="E52" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F52" s="2">
         <v>714</v>
       </c>
       <c r="G52" s="2">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H52" s="2" t="s">
         <v>25</v>
@@ -2744,51 +2757,51 @@
       </c>
       <c r="K52">
         <f>E52*(1000/F52)</f>
-        <v>5.6022408963585431</v>
+        <v>7.0028011204481793</v>
       </c>
       <c r="L52">
         <f>K52/D52</f>
-        <v>8.4882437823614286E-3</v>
+        <v>1.0610304727951787E-2</v>
       </c>
       <c r="N52">
         <f>AA50/K52</f>
-        <v>2.4990000000000001</v>
+        <v>1.9992000000000001</v>
       </c>
       <c r="O52">
         <f>AA51/K52</f>
-        <v>6.2475000000000005</v>
+        <v>4.9980000000000002</v>
       </c>
       <c r="P52">
         <f>AA52/K52</f>
-        <v>17.850000000000001</v>
+        <v>14.28</v>
       </c>
       <c r="Q52">
         <f>AA53/(K52/3)</f>
-        <v>10.71</v>
+        <v>8.5679999999999996</v>
       </c>
       <c r="R52">
         <f>AA54/K52</f>
-        <v>8.0325000000000006</v>
+        <v>6.4260000000000002</v>
       </c>
       <c r="S52">
         <f>AA55/K52</f>
-        <v>26.775000000000002</v>
+        <v>21.42</v>
       </c>
       <c r="T52">
         <f>AA56/(K52/3)</f>
-        <v>10.71</v>
+        <v>8.5679999999999996</v>
       </c>
       <c r="U52">
         <f>AA57/(K52/3)</f>
-        <v>13.387500000000001</v>
+        <v>10.709999999999999</v>
       </c>
       <c r="V52">
         <f>AA58/K52</f>
-        <v>44.625</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="W52">
         <f>AA59/(K52/3)</f>
-        <v>18.742500000000003</v>
+        <v>14.994</v>
       </c>
       <c r="Z52" s="2" t="s">
         <v>33</v>
@@ -2819,13 +2832,13 @@
         <v>980</v>
       </c>
       <c r="E53" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F53" s="2">
         <v>625</v>
       </c>
       <c r="G53" s="2">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>25</v>
@@ -2835,51 +2848,51 @@
       </c>
       <c r="K53">
         <f>E53*(1000/F53)</f>
-        <v>8</v>
+        <v>9.6000000000000014</v>
       </c>
       <c r="L53">
         <f>K53/D53</f>
-        <v>8.1632653061224497E-3</v>
+        <v>9.79591836734694E-3</v>
       </c>
       <c r="N53">
         <f>AA50/K53</f>
-        <v>1.75</v>
+        <v>1.458333333333333</v>
       </c>
       <c r="O53">
         <f>AA51/K53</f>
-        <v>4.375</v>
+        <v>3.6458333333333326</v>
       </c>
       <c r="P53">
         <f>AA52/K53</f>
-        <v>12.5</v>
+        <v>10.416666666666664</v>
       </c>
       <c r="Q53">
         <f>AA53/(K53/3)</f>
-        <v>7.5</v>
+        <v>6.2499999999999991</v>
       </c>
       <c r="R53">
         <f>AA54/K53</f>
-        <v>5.625</v>
+        <v>4.6874999999999991</v>
       </c>
       <c r="S53">
         <f>AA55/K53</f>
-        <v>18.75</v>
+        <v>15.624999999999998</v>
       </c>
       <c r="T53">
         <f>AA56/(K53/3)</f>
-        <v>7.5</v>
+        <v>6.2499999999999991</v>
       </c>
       <c r="U53">
         <f>AA57/(K53/3)</f>
-        <v>9.375</v>
+        <v>7.8124999999999982</v>
       </c>
       <c r="V53">
         <f>AA58/K53</f>
-        <v>31.25</v>
+        <v>26.041666666666664</v>
       </c>
       <c r="W53">
         <f>AA59/(K53/3)</f>
-        <v>13.125</v>
+        <v>10.937499999999998</v>
       </c>
       <c r="Z53" s="2" t="s">
         <v>34</v>
@@ -2910,13 +2923,13 @@
         <v>1350</v>
       </c>
       <c r="E54" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F54" s="2">
         <v>555</v>
       </c>
       <c r="G54" s="2">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>25</v>
@@ -2926,51 +2939,51 @@
       </c>
       <c r="K54">
         <f>E54*(1000/F54)</f>
-        <v>10.810810810810811</v>
+        <v>12.612612612612613</v>
       </c>
       <c r="L54">
         <f>K54/D54</f>
-        <v>8.0080080080080079E-3</v>
+        <v>9.3426760093426771E-3</v>
       </c>
       <c r="N54">
         <f>AA50/K54</f>
-        <v>1.2949999999999999</v>
+        <v>1.1099999999999999</v>
       </c>
       <c r="O54">
         <f>AA51/K54</f>
-        <v>3.2375000000000003</v>
+        <v>2.7749999999999999</v>
       </c>
       <c r="P54">
         <f>AA52/K54</f>
-        <v>9.25</v>
+        <v>7.9285714285714279</v>
       </c>
       <c r="Q54">
         <f>AA53/(K54/3)</f>
-        <v>5.55</v>
+        <v>4.7571428571428571</v>
       </c>
       <c r="R54">
         <f>AA54/K54</f>
-        <v>4.1625000000000005</v>
+        <v>3.5678571428571426</v>
       </c>
       <c r="S54">
         <f>AA55/K54</f>
-        <v>13.875</v>
+        <v>11.892857142857142</v>
       </c>
       <c r="T54">
         <f>AA56/(K54/3)</f>
-        <v>5.55</v>
+        <v>4.7571428571428571</v>
       </c>
       <c r="U54">
         <f>AA57/(K54/3)</f>
-        <v>6.9375</v>
+        <v>5.9464285714285712</v>
       </c>
       <c r="V54">
         <f>AA58/K54</f>
-        <v>23.125</v>
+        <v>19.821428571428569</v>
       </c>
       <c r="W54">
         <f>AA59/(K54/3)</f>
-        <v>9.7125000000000004</v>
+        <v>8.3249999999999993</v>
       </c>
       <c r="Z54" s="2" t="s">
         <v>35</v>
@@ -3412,7 +3425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H1048576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B15"/>
     </sheetView>
   </sheetViews>
@@ -3977,8 +3990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4568,7 +4581,7 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C36">
         <v>12</v>

</xml_diff>